<commit_message>
Kevin: Created CombineCSVs2 to TryCatch Excel errors
</commit_message>
<xml_diff>
--- a/output/Bids.xlsx
+++ b/output/Bids.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6431dddeb4959f/Documents/UiPath/Diamond/Project1/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project1\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="109_{0D15760E-0516-437A-8A7A-22C9E57F39AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A79C7E22-4BB5-4B74-B801-CE1F2F2C07CB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Awarded" sheetId="3" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OpenBids!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Top5'!$A$1:$P$49</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="108">
   <si>
     <t>Quote</t>
   </si>
@@ -128,419 +127,267 @@
     <t>UOM</t>
   </si>
   <si>
-    <t>MOESCHETQ22001771</t>
-  </si>
-  <si>
     <t>Quotation</t>
   </si>
   <si>
-    <t>FHSS - ECG Day 2022 Self Profiling for Secondary 4 and 5 students</t>
-  </si>
-  <si>
     <t>Ministry of Education - Schools</t>
   </si>
   <si>
-    <t>13 Apr 2022 01:49PM</t>
-  </si>
-  <si>
-    <t>22 Apr 2022 01:00PM</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>MISS SITI ROHANI HANIM BINTE SELAMAT</t>
-  </si>
-  <si>
-    <t>siti_rohani_hanim_selamat@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>5 Jurong West Street 41, Singapore 649410</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001765</t>
-  </si>
-  <si>
-    <t>Supply of Instructors for Provision of English Debate Programme in Jurong Secondary School.</t>
-  </si>
-  <si>
-    <t>13 Apr 2022 01:05PM</t>
-  </si>
-  <si>
-    <t>MS SUTHA RAJASEKARAN</t>
-  </si>
-  <si>
-    <t>sutha_rajasekaran@schools.gov.sg</t>
-  </si>
-  <si>
-    <t>31 Yuan Ching Road
-Singapore 618652</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001767</t>
-  </si>
-  <si>
-    <t>SUPPLY OF INSTRUCTORS FOR SPEECH AND DRAMA PROGRAMME, GEYLANG METHODIST SCHOOL (PRIMARY)</t>
-  </si>
-  <si>
-    <t>13 Apr 2022 12:50PM</t>
-  </si>
-  <si>
-    <t>MRS TAN-LIM SIEW KUAN</t>
-  </si>
-  <si>
-    <t>lim_siew_kuan@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>4 GEYLANG EAST CENTRAL SINGAPORE 389706</t>
-  </si>
-  <si>
-    <t>NYP000ETQ22000080</t>
-  </si>
-  <si>
-    <t>NYP000ETQ22000080 / AOR2201281P</t>
-  </si>
-  <si>
-    <t>Invitation to Quote for the Provision of Virtual Innovation and Enterprise Booster-1 programme For NYP Learners</t>
-  </si>
-  <si>
     <t>Nanyang Polytechnic</t>
   </si>
   <si>
-    <t>13 Apr 2022 12:20PM</t>
-  </si>
-  <si>
-    <t>KEN LIM</t>
-  </si>
-  <si>
-    <t>ken_lim@nyp.edu.sg</t>
-  </si>
-  <si>
-    <t>6550 0516</t>
-  </si>
-  <si>
-    <t>Nanyang Polytechnic, 180 Ang Mo Kio Ave 8, Singapore 569830</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001758</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001758 / Level Camp/2022/02</t>
-  </si>
-  <si>
-    <t>Provision of instructors, equipment and venues (venues for water-based activities only) for 3 Days Non-Residential Secondary 2 Outdoor Adventure Camp</t>
-  </si>
-  <si>
-    <t>13 Apr 2022 10:20AM</t>
-  </si>
-  <si>
     <t>25 Apr 2022 01:00PM</t>
   </si>
   <si>
-    <t>TAN WEE HIAN</t>
-  </si>
-  <si>
-    <t>TAN_Wee_Hian@schools.gov.sg</t>
-  </si>
-  <si>
-    <t>CHIJ Katong Convent
-346 Marine Terrace
-Singapore 449150</t>
-  </si>
-  <si>
-    <t>YRS000ETT22000001</t>
-  </si>
-  <si>
-    <t>YRS000ETT22000001 / YRSG/T02/2022</t>
-  </si>
-  <si>
-    <t>Tender</t>
-  </si>
-  <si>
-    <t>Provision of training in Employability Skills, Digital Literacy and Workplace Literacy</t>
-  </si>
-  <si>
-    <t>Yellow Ribbon Singapore</t>
-  </si>
-  <si>
-    <t>12 Apr 2022 06:35PM</t>
-  </si>
-  <si>
-    <t>06 May 2022 04:00PM</t>
-  </si>
-  <si>
-    <t>FAEZAH BINTE RADIMAN</t>
-  </si>
-  <si>
-    <t>Faezah_Radiman@yellowribbon.gov.sg</t>
-  </si>
-  <si>
-    <t>980 Upper Changi Road North, S507708</t>
-  </si>
-  <si>
-    <t>MOE000ETQ22000102</t>
-  </si>
-  <si>
-    <t>Provision of Facilitator/s to coach and train  MOE Language Centre Key Personnels(KPs) and Staff in a series Leadership and Professional Programmes</t>
-  </si>
-  <si>
-    <t>Ministry of Education</t>
-  </si>
-  <si>
-    <t>12 Apr 2022 06:05PM</t>
-  </si>
-  <si>
     <t>04 May 2022 01:00PM</t>
   </si>
   <si>
-    <t>TAN LAI ENG</t>
-  </si>
-  <si>
-    <t>tan_lai_eng@schools.gov.sg</t>
-  </si>
-  <si>
-    <t>11, Bishan Street 14 Singapore 579782</t>
-  </si>
-  <si>
-    <t>FOR000ETQ22000019</t>
-  </si>
-  <si>
-    <t>Provision of Hebrew language training for 3 MFA officers in Tel Aviv</t>
-  </si>
-  <si>
-    <t>Ministry of Foreign Affairs</t>
-  </si>
-  <si>
-    <t>12 Apr 2022 04:35PM</t>
-  </si>
-  <si>
-    <t>26 Apr 2022 01:00PM</t>
-  </si>
-  <si>
-    <t>NARELLE LEE SALIKIN</t>
-  </si>
-  <si>
-    <t>Narelle_Lee_Salikin@mfa.gov.sg</t>
-  </si>
-  <si>
-    <t>1 Sherwood Road, Tanglin</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001729</t>
-  </si>
-  <si>
-    <t>Supply of Instructors for Provision of 3-Day Secondary 1 Outdoor Adventure Camp (Non-Residential) for West Spring Secondary School</t>
-  </si>
-  <si>
-    <t>21 Apr 2022 01:00PM</t>
-  </si>
-  <si>
-    <t>MR FAURONI SUKHAIMI</t>
-  </si>
-  <si>
-    <t>nai_wee_beng@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>West Spring Secondary School, 61 Senja Road, Singapore 677737</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001745</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001745 / AOR2022/161(DesignThinking_P4)</t>
-  </si>
-  <si>
-    <t>Instructors for Design Thinking Workshop for P4 Students in Yangzheng Pri School</t>
-  </si>
-  <si>
-    <t>MDM LASIME KUMARI</t>
-  </si>
-  <si>
-    <t>lasime_kumari@schools.gov.sg</t>
-  </si>
-  <si>
-    <t>15 Serangoon Avenue 3, Singapore 556108</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001740</t>
-  </si>
-  <si>
-    <t>2 DAYS STUDENTS LEADERS' TRAINING PROGRAMME</t>
-  </si>
-  <si>
-    <t>MS LIAW HSIAO-MEIN</t>
-  </si>
-  <si>
-    <t>liaw_hsiao_mein@schools.gov.sg</t>
-  </si>
-  <si>
-    <t>3 Yishun Ring Road
-S(768675)</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
-    <t>MOESCHETQ22001441</t>
-  </si>
-  <si>
-    <t>ST ANDREWS JUNIOR SCHOOL: LANGUAGE FACILITATOR FOR DYSLEXIA INTERVENTION 2022-2024</t>
-  </si>
-  <si>
-    <t>ONG POH HWEE</t>
-  </si>
-  <si>
-    <t>17,745.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001431 / MOESCHEAR22010448 (AOR2022107)</t>
-  </si>
-  <si>
-    <t>Lifeskills Workshop 2022 for P1, P2 and P3 Students, Yangzheng Pri School</t>
-  </si>
-  <si>
-    <t>EKA TRAINING GROUP PTE. LTD.</t>
-  </si>
-  <si>
-    <t>14,222.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001375 / 2022-CCAVB--1</t>
-  </si>
-  <si>
-    <t>Supply of Instructor for Volleyball CCA Training Programme in Cantonment Primary School</t>
-  </si>
-  <si>
-    <t>MINTONETTE SPORTS MANAGEMENT</t>
-  </si>
-  <si>
-    <t>9,100.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001386</t>
-  </si>
-  <si>
-    <t>Rulang Primary School is looking for a vendor to supply, deliver, assemble and install one unit of Active Floor System - 2022</t>
-  </si>
-  <si>
-    <t>EDN LEARNING DISCOVERIES PTE. LTD.</t>
-  </si>
-  <si>
-    <t>12,980.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001362</t>
-  </si>
-  <si>
-    <t>Supply of Instructor for Student Leader Workshop for Primary 4 Prefects in South View Primary School.</t>
-  </si>
-  <si>
-    <t>ADAM KHOO LIFE SKILLS COMPANY PTE. LTD.</t>
-  </si>
-  <si>
-    <t>3,750.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001335</t>
-  </si>
-  <si>
-    <t>Supply of Instructors for provision of 3-Day non-residential Primary 5 Outdoor and Leadership Adventure Camp for Pei Chun Public School (2022)</t>
-  </si>
-  <si>
-    <t>TOUCH COMMUNITY SERVICES LIMITED</t>
-  </si>
-  <si>
-    <t>23,162.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001322 / JYSS0102022</t>
-  </si>
-  <si>
-    <t>ITQ FOR SUPPLY AND DELIVERY OF SCHOOL OPERATION SERVICE ROBOTS (2 UNITS) FOR JUYING SECONDARY SCHOOL.</t>
-  </si>
-  <si>
-    <t>ROBOSOLUTIONS PTE. LTD.</t>
-  </si>
-  <si>
-    <t>17,000.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001316</t>
-  </si>
-  <si>
-    <t>After School Programme in Kranji Secondary School</t>
-  </si>
-  <si>
-    <t>WOMEN'S INSTITUTE OF MANAGEMENT</t>
-  </si>
-  <si>
-    <t>6,185.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001306</t>
-  </si>
-  <si>
-    <t>Supply of Consultant/Trainer for Organisational Change Professional Developmental Programme in Poi Ching School</t>
-  </si>
-  <si>
-    <t>YI CONSULTANCY PTE. LTD.</t>
-  </si>
-  <si>
-    <t>45,200.00 (SGD)</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001299</t>
-  </si>
-  <si>
-    <t>Supply of Instructors for Coding Programme for P3 Students for Zhangde Primary School</t>
-  </si>
-  <si>
-    <t>DUCK LEARNING</t>
-  </si>
-  <si>
-    <t>5,125.00 (SGD)</t>
-  </si>
-  <si>
     <t>Download Link</t>
   </si>
   <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001771</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001765</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001767</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\NYP000ETQ22000080</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001758</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\YRS000ETT22000001</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOE000ETQ22000102</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\FOR000ETQ22000019</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001729</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001745</t>
-  </si>
-  <si>
-    <t>C:\Users\ryant.DESKTOP-P30VL9L\OneDrive\Documents\UiPath\Diamond\Project1\output\OPEN\MOESCHETQ22001740</t>
+    <t>MOESCHETQ22001816</t>
+  </si>
+  <si>
+    <t>Instructors for Digital Literacy Programme in Queenstown Secondary School</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 05:50PM</t>
+  </si>
+  <si>
+    <t>MR JOSEPH TEO</t>
+  </si>
+  <si>
+    <t>teo_chai_hong_joseph@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>1 Strathmore Road Singapore 148800</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001816</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001800</t>
+  </si>
+  <si>
+    <t>2022 English Bridging Support</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 05:05PM</t>
+  </si>
+  <si>
+    <t>GOH PAI SHEN</t>
+  </si>
+  <si>
+    <t>goh_pai_shen@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>Catholic High School (Secondary), 9 Bishan Street 22 Singapore 579767</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001800</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001802</t>
+  </si>
+  <si>
+    <t>ITQ for Supply of Instructor for Mother Tongue Fortnight activities for Students in Beacon Primary School for our P1-P6 students</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 04:05PM</t>
+  </si>
+  <si>
+    <t>MS LEE PEI PEI</t>
+  </si>
+  <si>
+    <t>lee_pei_pei@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>Ministry of Education,1, North Buona Vista Drive</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001802</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001811</t>
+  </si>
+  <si>
+    <t>Supply of Pianist for Choir CCA Programme in Clementi Primary School</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 03:35PM</t>
+  </si>
+  <si>
+    <t>FIONA KWAN</t>
+  </si>
+  <si>
+    <t>fiona_kwan_lok_mun@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>8 Clementi Avenue 3 Singapore 129903</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001811</t>
+  </si>
+  <si>
+    <t>NYP000ETQ22000081</t>
+  </si>
+  <si>
+    <t>To appoint training service providers for the provision of services to develop and deliver Masterclass Programmes for a period of 2 years</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 02:19PM</t>
+  </si>
+  <si>
+    <t>05 May 2022 01:00PM</t>
+  </si>
+  <si>
+    <t>JENNY LING / PATRICK PNG</t>
+  </si>
+  <si>
+    <t>jenny_ling@sirs.edu.sg</t>
+  </si>
+  <si>
+    <t>64173650 / 65500717</t>
+  </si>
+  <si>
+    <t>Singapore Institute of Retail Studies, 11 Eunos Road 8, Lifelong Learning Institute, #08-02/03/04, Singapore 408601</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\NYP000ETQ22000081</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001805</t>
+  </si>
+  <si>
+    <t>Manpower service for Science Lab 1+1 year</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 02:05PM</t>
+  </si>
+  <si>
+    <t>MRS EMILY WONG</t>
+  </si>
+  <si>
+    <t>fang_yoke_cheng_emily@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>90 Bukit Batok East Ave 6 S659762</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001805</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001795</t>
+  </si>
+  <si>
+    <t>Provision of 3 Days Non-Residential Primary 5 Cohort Outdoor Learning Camp 2022</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 01:04PM</t>
+  </si>
+  <si>
+    <t>RYAN TAY EN HUANG</t>
+  </si>
+  <si>
+    <t>ryan_tay_en_huang@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>Holy Innocents' Primary School
+5 Lorong Low Koon
+Singapore 536451</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001795</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001769</t>
+  </si>
+  <si>
+    <t>Primary 1 and Primary 2 Chinese Weiqi Enrichment Programme in Holy Innocents' Primary School</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 09:50AM</t>
+  </si>
+  <si>
+    <t>LEE SIEW KIAN JOYCE</t>
+  </si>
+  <si>
+    <t>lee_siew_kian_joyce@schools.gov.sg</t>
+  </si>
+  <si>
+    <t>Holy Innocents' Primary School
+5 Lorong Low Koon</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001769</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001791</t>
+  </si>
+  <si>
+    <t>Supply of Instructor for Student Leadership Programme for CHIJ (Katong) Primary: - P4 to P6 Prefects (Trainee &amp; Senior) and P3 to P6 Class Monitors</t>
+  </si>
+  <si>
+    <t>MR EDWARD TOH</t>
+  </si>
+  <si>
+    <t>toh_boon_how@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>CHIJ (KATONG) PRIMARY
+17 MARTIA ROAD
+SINGAPORE 424821</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001791</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001788</t>
+  </si>
+  <si>
+    <t>Supply of Instructors for Student Leadership Training Programme in Pioneer Primary School</t>
+  </si>
+  <si>
+    <t>MOHAMED ASHIQ S/O AMEERDEEN M</t>
+  </si>
+  <si>
+    <t>mohamed_ashiq_ameerdeen_m@schools.gov.sg</t>
+  </si>
+  <si>
+    <t>Pioneer primary school, 31 Jurong West St 91, S649037</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001788</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001730</t>
+  </si>
+  <si>
+    <t>Supply of Instructors for Primary 1 Programme for Active Learning (PAL) - Dance Module in Peiying Primary School</t>
+  </si>
+  <si>
+    <t>MR MOHAMAD IKHWAN BIN MOHAMAD HARON</t>
+  </si>
+  <si>
+    <t>mohamad_ikhwan_mohamad_haron@schools.gov.sg</t>
+  </si>
+  <si>
+    <t>Peiying Primary School, 651 Yishun Ring Road, S768687</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001730</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -889,6 +736,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,6 +850,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1025,34 +876,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="131"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,34 +918,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="131"/>
                 <c:pt idx="0">
-                  <c:v>382</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>365</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>286</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>199</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>189</c:v>
+                  <c:v>371</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>69</c:v>
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1671,6 +1528,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1678,7 +1536,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill>
@@ -2619,21 +2476,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876A7BC6-4E87-4806-AC09-A14CCBAD7662}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="35.7265625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="4" width="8.77734375" style="1"/>
+    <col min="5" max="5" width="35.77734375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2651,206 +2508,6 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2859,28 +2516,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39582A0F-F993-4278-A272-EAB12E1434D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="8.90625" style="1" customWidth="1"/>
-    <col min="4" max="8" width="8.7265625" style="1"/>
-    <col min="9" max="9" width="6.08984375" style="1" customWidth="1"/>
-    <col min="10" max="13" width="8.7265625" style="1"/>
-    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" customWidth="1"/>
+    <col min="4" max="8" width="8.77734375" style="1"/>
+    <col min="9" max="9" width="6.109375" style="1" customWidth="1"/>
+    <col min="10" max="13" width="8.77734375" style="1"/>
+    <col min="14" max="16" width="14.77734375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2930,404 +2585,401 @@
         <v>23</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="1">
+        <v>64741055</v>
+      </c>
+      <c r="M2" s="1">
+        <v>64741295</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="1">
+        <v>31</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="1">
-        <v>65633067</v>
-      </c>
-      <c r="M2" s="1">
-        <v>65634379</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="1">
-        <v>365</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="1">
+        <v>64582177</v>
+      </c>
+      <c r="M3" s="1">
+        <v>64561322</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="1">
+        <v>345</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="1">
-        <v>62655980</v>
-      </c>
-      <c r="M3" s="1">
-        <v>62686414</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="1">
-        <v>69</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="1">
+        <v>67697255</v>
+      </c>
+      <c r="M4" s="1">
+        <v>67697244</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="1">
+        <v>395</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="1">
-        <v>67486746</v>
-      </c>
-      <c r="M4" s="1">
-        <v>67488980</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="1">
-        <v>55</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="1">
+        <v>67797449</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="1">
+        <v>255</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O5" s="1">
-        <v>382</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q5" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="1">
+        <v>358</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="1">
-        <v>64423482</v>
-      </c>
-      <c r="M6" s="1">
-        <v>64494405</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="1">
-        <v>286</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="1">
+        <v>68962054</v>
+      </c>
+      <c r="M7" s="1">
+        <v>65632356</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="1">
+        <v>154</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" s="1">
-        <v>62142839</v>
-      </c>
-      <c r="M7" s="1">
-        <v>65467441</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="1">
-        <v>189</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q7" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="1">
+        <v>62886516</v>
+      </c>
+      <c r="M8" s="1">
+        <v>62876393</v>
+      </c>
+      <c r="N8" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" s="52">
+        <v>335</v>
+      </c>
+      <c r="P8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8" s="1">
-        <v>62587794</v>
-      </c>
-      <c r="M8" s="1">
-        <v>62583913</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8" s="1">
-        <v>250</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q8" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>86</v>
@@ -3336,51 +2988,51 @@
         <v>87</v>
       </c>
       <c r="L9" s="1">
-        <v>63797788</v>
+        <v>62886516</v>
       </c>
       <c r="M9" s="1">
-        <v>63797997</v>
-      </c>
-      <c r="N9" s="1" t="s">
+        <v>62876393</v>
+      </c>
+      <c r="N9" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="O9" s="1">
-        <v>77</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>106</v>
+      <c r="O9" s="52">
+        <v>371</v>
+      </c>
+      <c r="P9" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>92</v>
@@ -3389,51 +3041,51 @@
         <v>93</v>
       </c>
       <c r="L10" s="1">
-        <v>68920369</v>
+        <v>63443072</v>
       </c>
       <c r="M10" s="1">
-        <v>68929468</v>
-      </c>
-      <c r="N10" s="1" t="s">
+        <v>63459007</v>
+      </c>
+      <c r="N10" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="O10" s="1">
-        <v>240</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>106</v>
+      <c r="O10" s="52">
+        <v>83</v>
+      </c>
+      <c r="P10" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>98</v>
@@ -3442,75 +3094,72 @@
         <v>99</v>
       </c>
       <c r="L11" s="1">
-        <v>62846298</v>
-      </c>
-      <c r="M11" s="1">
-        <v>62879778</v>
+        <v>67932039</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>100</v>
       </c>
       <c r="O11" s="1">
-        <v>199</v>
+        <v>399</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" s="1">
+        <v>62575684</v>
+      </c>
+      <c r="M12" s="1">
+        <v>67558802</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O12" s="1">
+        <v>227</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L12" s="1">
-        <v>62579873</v>
-      </c>
-      <c r="M12" s="1">
-        <v>62574373</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O12" s="1">
-        <v>265</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3519,21 +3168,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5E9977-255A-404F-9037-914CC69CEAF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="8.7265625" style="1"/>
-    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="13" width="8.77734375" style="1"/>
+    <col min="14" max="14" width="14.77734375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3583,559 +3232,587 @@
         <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>64741055</v>
+      </c>
+      <c r="M2">
+        <v>64741295</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3">
+        <v>64582177</v>
+      </c>
+      <c r="M3">
+        <v>64561322</v>
+      </c>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3">
+        <v>345</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>67697255</v>
+      </c>
+      <c r="M4">
+        <v>67697244</v>
+      </c>
+      <c r="N4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4">
+        <v>395</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5">
+        <v>67797449</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5">
+        <v>255</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6">
+        <v>358</v>
+      </c>
+      <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7">
+        <v>68962054</v>
+      </c>
+      <c r="M7">
+        <v>65632356</v>
+      </c>
+      <c r="N7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7">
+        <v>154</v>
+      </c>
+      <c r="P7" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2"/>
-      <c r="N2" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2">
-        <v>382</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8">
+        <v>62886516</v>
+      </c>
+      <c r="M8">
+        <v>62876393</v>
+      </c>
+      <c r="N8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8">
+        <v>335</v>
+      </c>
+      <c r="P8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9">
+        <v>62886516</v>
+      </c>
+      <c r="M9">
+        <v>62876393</v>
+      </c>
+      <c r="N9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O9">
+        <v>371</v>
+      </c>
+      <c r="P9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10">
+        <v>63443072</v>
+      </c>
+      <c r="M10">
+        <v>63459007</v>
+      </c>
+      <c r="N10" t="s">
+        <v>94</v>
+      </c>
+      <c r="O10">
+        <v>83</v>
+      </c>
+      <c r="P10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11">
+        <v>67932039</v>
+      </c>
+      <c r="M11"/>
+      <c r="N11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>399</v>
+      </c>
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12">
+        <v>62575684</v>
+      </c>
+      <c r="M12">
+        <v>67558802</v>
+      </c>
+      <c r="N12" t="s">
         <v>106</v>
       </c>
-      <c r="Q2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="O12">
+        <v>227</v>
+      </c>
+      <c r="P12" t="s">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3">
-        <v>65633067</v>
-      </c>
-      <c r="M3">
-        <v>65634379</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3">
-        <v>365</v>
-      </c>
-      <c r="P3" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4">
-        <v>64423482</v>
-      </c>
-      <c r="M4">
-        <v>64494405</v>
-      </c>
-      <c r="N4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4">
-        <v>286</v>
-      </c>
-      <c r="P4" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K5" t="s">
-        <v>104</v>
-      </c>
-      <c r="L5">
-        <v>62579873</v>
-      </c>
-      <c r="M5">
-        <v>62574373</v>
-      </c>
-      <c r="N5" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5">
-        <v>265</v>
-      </c>
-      <c r="P5" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6">
-        <v>62587794</v>
-      </c>
-      <c r="M6">
-        <v>62583913</v>
-      </c>
-      <c r="N6" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6">
-        <v>250</v>
-      </c>
-      <c r="P6" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K7" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7">
-        <v>68920369</v>
-      </c>
-      <c r="M7">
-        <v>68929468</v>
-      </c>
-      <c r="N7" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7">
-        <v>240</v>
-      </c>
-      <c r="P7" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>98</v>
-      </c>
-      <c r="K8" t="s">
-        <v>99</v>
-      </c>
-      <c r="L8">
-        <v>62846298</v>
-      </c>
-      <c r="M8">
-        <v>62879778</v>
-      </c>
-      <c r="N8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O8">
-        <v>199</v>
-      </c>
-      <c r="P8" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" t="s">
-        <v>71</v>
-      </c>
-      <c r="L9">
-        <v>62142839</v>
-      </c>
-      <c r="M9">
-        <v>65467441</v>
-      </c>
-      <c r="N9" t="s">
-        <v>72</v>
-      </c>
-      <c r="O9">
-        <v>189</v>
-      </c>
-      <c r="P9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" t="s">
-        <v>87</v>
-      </c>
-      <c r="L10">
-        <v>63797788</v>
-      </c>
-      <c r="M10">
-        <v>63797997</v>
-      </c>
-      <c r="N10" t="s">
-        <v>88</v>
-      </c>
-      <c r="O10">
-        <v>77</v>
-      </c>
-      <c r="P10" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11">
-        <v>62655980</v>
-      </c>
-      <c r="M11">
-        <v>62686414</v>
-      </c>
-      <c r="N11" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11">
-        <v>69</v>
-      </c>
-      <c r="P11" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
       <c r="Q12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -4153,7 +3830,7 @@
       <c r="O13"/>
       <c r="P13"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -4171,7 +3848,7 @@
       <c r="O14"/>
       <c r="P14"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -4189,7 +3866,7 @@
       <c r="O15"/>
       <c r="P15"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -4207,7 +3884,7 @@
       <c r="O16"/>
       <c r="P16"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -4225,7 +3902,7 @@
       <c r="O17"/>
       <c r="P17"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -4243,7 +3920,7 @@
       <c r="O18"/>
       <c r="P18"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -4261,7 +3938,7 @@
       <c r="O19"/>
       <c r="P19"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -4279,7 +3956,7 @@
       <c r="O20"/>
       <c r="P20"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -4297,7 +3974,7 @@
       <c r="O21"/>
       <c r="P21"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -4315,7 +3992,7 @@
       <c r="O22"/>
       <c r="P22"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -4333,7 +4010,7 @@
       <c r="O23"/>
       <c r="P23"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -4351,7 +4028,7 @@
       <c r="O24"/>
       <c r="P24"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -4369,7 +4046,7 @@
       <c r="O25"/>
       <c r="P25"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -4387,7 +4064,7 @@
       <c r="O26"/>
       <c r="P26"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -4405,7 +4082,7 @@
       <c r="O27"/>
       <c r="P27"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -4423,7 +4100,7 @@
       <c r="O28"/>
       <c r="P28"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -4441,7 +4118,7 @@
       <c r="O29"/>
       <c r="P29"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -4459,7 +4136,7 @@
       <c r="O30"/>
       <c r="P30"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -4477,7 +4154,7 @@
       <c r="O31"/>
       <c r="P31"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -4495,7 +4172,7 @@
       <c r="O32"/>
       <c r="P32"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -4513,7 +4190,7 @@
       <c r="O33"/>
       <c r="P33"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -4531,7 +4208,7 @@
       <c r="O34"/>
       <c r="P34"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -4549,7 +4226,7 @@
       <c r="O35"/>
       <c r="P35"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -4567,7 +4244,7 @@
       <c r="O36"/>
       <c r="P36"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -4585,7 +4262,7 @@
       <c r="O37"/>
       <c r="P37"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -4603,7 +4280,7 @@
       <c r="O38"/>
       <c r="P38"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -4621,7 +4298,7 @@
       <c r="O39"/>
       <c r="P39"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -4639,7 +4316,7 @@
       <c r="O40"/>
       <c r="P40"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -4657,7 +4334,7 @@
       <c r="O41"/>
       <c r="P41"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -4675,7 +4352,7 @@
       <c r="O42"/>
       <c r="P42"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -4693,7 +4370,7 @@
       <c r="O43"/>
       <c r="P43"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -4711,7 +4388,7 @@
       <c r="O44"/>
       <c r="P44"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -4729,7 +4406,7 @@
       <c r="O45"/>
       <c r="P45"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -4747,7 +4424,7 @@
       <c r="O46"/>
       <c r="P46"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -4765,7 +4442,7 @@
       <c r="O47"/>
       <c r="P47"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -4783,7 +4460,7 @@
       <c r="O48"/>
       <c r="P48"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -4801,7 +4478,7 @@
       <c r="O49"/>
       <c r="P49"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -4819,7 +4496,7 @@
       <c r="O50"/>
       <c r="P50"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -4837,7 +4514,7 @@
       <c r="O51"/>
       <c r="P51"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -4855,7 +4532,7 @@
       <c r="O52"/>
       <c r="P52"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -4873,7 +4550,7 @@
       <c r="O53"/>
       <c r="P53"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -4891,7 +4568,7 @@
       <c r="O54"/>
       <c r="P54"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -4909,7 +4586,7 @@
       <c r="O55"/>
       <c r="P55"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -4927,7 +4604,7 @@
       <c r="O56"/>
       <c r="P56"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -4945,7 +4622,7 @@
       <c r="O57"/>
       <c r="P57"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -4963,7 +4640,7 @@
       <c r="O58"/>
       <c r="P58"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -4981,7 +4658,7 @@
       <c r="O59"/>
       <c r="P59"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -4999,7 +4676,7 @@
       <c r="O60"/>
       <c r="P60"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -5017,7 +4694,7 @@
       <c r="O61"/>
       <c r="P61"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -5035,7 +4712,7 @@
       <c r="O62"/>
       <c r="P62"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -5053,7 +4730,7 @@
       <c r="O63"/>
       <c r="P63"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -5071,7 +4748,7 @@
       <c r="O64"/>
       <c r="P64"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -5089,7 +4766,7 @@
       <c r="O65"/>
       <c r="P65"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -5107,7 +4784,7 @@
       <c r="O66"/>
       <c r="P66"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -5125,7 +4802,7 @@
       <c r="O67"/>
       <c r="P67"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -5143,7 +4820,7 @@
       <c r="O68"/>
       <c r="P68"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -5161,7 +4838,7 @@
       <c r="O69"/>
       <c r="P69"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -5179,7 +4856,7 @@
       <c r="O70"/>
       <c r="P70"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -5197,7 +4874,7 @@
       <c r="O71"/>
       <c r="P71"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -5215,7 +4892,7 @@
       <c r="O72"/>
       <c r="P72"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -5233,7 +4910,7 @@
       <c r="O73"/>
       <c r="P73"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -5251,7 +4928,7 @@
       <c r="O74"/>
       <c r="P74"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -5269,7 +4946,7 @@
       <c r="O75"/>
       <c r="P75"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -5287,7 +4964,7 @@
       <c r="O76"/>
       <c r="P76"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -5305,7 +4982,7 @@
       <c r="O77"/>
       <c r="P77"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -5323,7 +5000,7 @@
       <c r="O78"/>
       <c r="P78"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -5341,7 +5018,7 @@
       <c r="O79"/>
       <c r="P79"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -5359,7 +5036,7 @@
       <c r="O80"/>
       <c r="P80"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -5377,7 +5054,7 @@
       <c r="O81"/>
       <c r="P81"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -5395,7 +5072,7 @@
       <c r="O82"/>
       <c r="P82"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -5413,7 +5090,7 @@
       <c r="O83"/>
       <c r="P83"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -5431,7 +5108,7 @@
       <c r="O84"/>
       <c r="P84"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -5449,7 +5126,7 @@
       <c r="O85"/>
       <c r="P85"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -5467,7 +5144,7 @@
       <c r="O86"/>
       <c r="P86"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -5485,7 +5162,7 @@
       <c r="O87"/>
       <c r="P87"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -5503,7 +5180,7 @@
       <c r="O88"/>
       <c r="P88"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -5521,7 +5198,7 @@
       <c r="O89"/>
       <c r="P89"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -5539,7 +5216,7 @@
       <c r="O90"/>
       <c r="P90"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -5557,7 +5234,7 @@
       <c r="O91"/>
       <c r="P91"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -5575,7 +5252,7 @@
       <c r="O92"/>
       <c r="P92"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -5593,7 +5270,7 @@
       <c r="O93"/>
       <c r="P93"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -5611,7 +5288,7 @@
       <c r="O94"/>
       <c r="P94"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -5629,7 +5306,7 @@
       <c r="O95"/>
       <c r="P95"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -5647,7 +5324,7 @@
       <c r="O96"/>
       <c r="P96"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -5665,7 +5342,7 @@
       <c r="O97"/>
       <c r="P97"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -5683,7 +5360,7 @@
       <c r="O98"/>
       <c r="P98"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -5701,7 +5378,7 @@
       <c r="O99"/>
       <c r="P99"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -5719,7 +5396,7 @@
       <c r="O100"/>
       <c r="P100"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -5737,7 +5414,7 @@
       <c r="O101"/>
       <c r="P101"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -5755,7 +5432,7 @@
       <c r="O102"/>
       <c r="P102"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -5773,7 +5450,7 @@
       <c r="O103"/>
       <c r="P103"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -5791,7 +5468,7 @@
       <c r="O104"/>
       <c r="P104"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -5809,7 +5486,7 @@
       <c r="O105"/>
       <c r="P105"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -5827,7 +5504,7 @@
       <c r="O106"/>
       <c r="P106"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -5845,7 +5522,7 @@
       <c r="O107"/>
       <c r="P107"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -5863,7 +5540,7 @@
       <c r="O108"/>
       <c r="P108"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -5881,7 +5558,7 @@
       <c r="O109"/>
       <c r="P109"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -5899,7 +5576,7 @@
       <c r="O110"/>
       <c r="P110"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -5917,7 +5594,7 @@
       <c r="O111"/>
       <c r="P111"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -5935,7 +5612,7 @@
       <c r="O112"/>
       <c r="P112"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
@@ -5953,7 +5630,7 @@
       <c r="O113"/>
       <c r="P113"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -5971,7 +5648,7 @@
       <c r="O114"/>
       <c r="P114"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
@@ -5989,7 +5666,7 @@
       <c r="O115"/>
       <c r="P115"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -6007,7 +5684,7 @@
       <c r="O116"/>
       <c r="P116"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -6025,7 +5702,7 @@
       <c r="O117"/>
       <c r="P117"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -6043,7 +5720,7 @@
       <c r="O118"/>
       <c r="P118"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -6061,7 +5738,7 @@
       <c r="O119"/>
       <c r="P119"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -6079,7 +5756,7 @@
       <c r="O120"/>
       <c r="P120"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
@@ -6097,7 +5774,7 @@
       <c r="O121"/>
       <c r="P121"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
@@ -6115,7 +5792,7 @@
       <c r="O122"/>
       <c r="P122"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -6133,7 +5810,7 @@
       <c r="O123"/>
       <c r="P123"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
@@ -6151,7 +5828,7 @@
       <c r="O124"/>
       <c r="P124"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
@@ -6169,7 +5846,7 @@
       <c r="O125"/>
       <c r="P125"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
@@ -6187,7 +5864,7 @@
       <c r="O126"/>
       <c r="P126"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -6205,7 +5882,7 @@
       <c r="O127"/>
       <c r="P127"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
@@ -6223,7 +5900,7 @@
       <c r="O128"/>
       <c r="P128"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
@@ -6241,7 +5918,7 @@
       <c r="O129"/>
       <c r="P129"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -6259,7 +5936,7 @@
       <c r="O130"/>
       <c r="P130"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -6277,7 +5954,7 @@
       <c r="O131"/>
       <c r="P131"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -6285,7 +5962,7 @@
       <c r="E132"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q132">
+  <sortState ref="A2:Q132">
     <sortCondition descending="1" ref="O1:O132"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6293,19 +5970,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="46" x14ac:dyDescent="1">
+    <row r="2" spans="2:15" ht="46.2" x14ac:dyDescent="0.85">
       <c r="B2" s="38" t="s">
         <v>20</v>
       </c>
@@ -6323,7 +6000,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="4" spans="2:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="43" t="s">
         <v>2</v>
       </c>
@@ -6340,7 +6017,7 @@
       <c r="K4" s="50"/>
       <c r="L4" s="51"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -6351,7 +6028,7 @@
       <c r="K6" s="17"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
@@ -6362,7 +6039,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="2:15" ht="46" x14ac:dyDescent="1">
+    <row r="8" spans="2:15" ht="46.2" x14ac:dyDescent="0.85">
       <c r="B8" s="6"/>
       <c r="C8" s="9">
         <f>COUNT(OpenBids!A:A)</f>
@@ -6378,11 +6055,11 @@
       <c r="J8" s="19"/>
       <c r="K8" s="22">
         <f>COUNT(Awarded!A:A)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
@@ -6393,7 +6070,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
@@ -6404,14 +6081,14 @@
       <c r="K10" s="24"/>
       <c r="L10" s="25"/>
     </row>
-    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.3">
       <c r="B12" s="46" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="48"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="26" t="s">
         <v>5</v>
       </c>
@@ -6432,19 +6109,19 @@
       </c>
       <c r="L13" s="41"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="27">
         <f>'Top5'!A2</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14" s="28" t="str">
         <f>'Top5'!B2</f>
-        <v>NYP000ETQ22000080</v>
+        <v>MOESCHETQ22001816</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="35" t="str">
         <f>'Top5'!E2</f>
-        <v>Invitation to Quote for the Provision of Virtual Innovation and Enterprise Booster-1 programme For NYP Learners</v>
+        <v>Instructors for Digital Literacy Programme in Queenstown Secondary School</v>
       </c>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
@@ -6453,23 +6130,23 @@
       <c r="J14" s="37"/>
       <c r="K14" s="31" t="str">
         <f>'Top5'!H2</f>
-        <v>22 Apr 2022 01:00PM</v>
+        <v>25 Apr 2022 01:00PM</v>
       </c>
       <c r="L14" s="29"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="27">
         <f>'Top5'!A3</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="28" t="str">
         <f>'Top5'!B3</f>
-        <v>MOESCHETQ22001771</v>
+        <v>MOESCHETQ22001800</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="35" t="str">
         <f>'Top5'!E3</f>
-        <v>FHSS - ECG Day 2022 Self Profiling for Secondary 4 and 5 students</v>
+        <v>2022 English Bridging Support</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
@@ -6478,23 +6155,23 @@
       <c r="J15" s="37"/>
       <c r="K15" s="31" t="str">
         <f>'Top5'!H3</f>
-        <v>22 Apr 2022 01:00PM</v>
+        <v>25 Apr 2022 01:00PM</v>
       </c>
       <c r="L15" s="29"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="27">
         <f>'Top5'!A4</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="28" t="str">
         <f>'Top5'!B4</f>
-        <v>MOESCHETQ22001758</v>
+        <v>MOESCHETQ22001802</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="35" t="str">
         <f>'Top5'!E4</f>
-        <v>Provision of instructors, equipment and venues (venues for water-based activities only) for 3 Days Non-Residential Secondary 2 Outdoor Adventure Camp</v>
+        <v>ITQ for Supply of Instructor for Mother Tongue Fortnight activities for Students in Beacon Primary School for our P1-P6 students</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -6507,19 +6184,19 @@
       </c>
       <c r="L16" s="29"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="27">
         <f>'Top5'!A5</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C17" s="28" t="str">
         <f>'Top5'!B5</f>
-        <v>MOESCHETQ22001740</v>
+        <v>MOESCHETQ22001811</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="35" t="str">
         <f>'Top5'!E5</f>
-        <v>2 DAYS STUDENTS LEADERS' TRAINING PROGRAMME</v>
+        <v>Supply of Pianist for Choir CCA Programme in Clementi Primary School</v>
       </c>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -6528,23 +6205,23 @@
       <c r="J17" s="37"/>
       <c r="K17" s="31" t="str">
         <f>'Top5'!H5</f>
-        <v>21 Apr 2022 01:00PM</v>
+        <v>25 Apr 2022 01:00PM</v>
       </c>
       <c r="L17" s="29"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="27">
         <f>'Top5'!A6</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" s="28" t="str">
         <f>'Top5'!B6</f>
-        <v>MOE000ETQ22000102</v>
+        <v>NYP000ETQ22000081</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="32" t="str">
         <f>'Top5'!E6</f>
-        <v>Provision of Facilitator/s to coach and train  MOE Language Centre Key Personnels(KPs) and Staff in a series Leadership and Professional Programmes</v>
+        <v>To appoint training service providers for the provision of services to develop and deliver Masterclass Programmes for a period of 2 years</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
@@ -6553,11 +6230,11 @@
       <c r="J18" s="34"/>
       <c r="K18" s="31" t="str">
         <f>'Top5'!H6</f>
-        <v>04 May 2022 01:00PM</v>
+        <v>05 May 2022 01:00PM</v>
       </c>
       <c r="L18" s="29"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>

</xml_diff>

<commit_message>
update combineCsvs to delete column Q row 12 beyond.
</commit_message>
<xml_diff>
--- a/output/Bids.xlsx
+++ b/output/Bids.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project1\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6431dddeb4959f/Documents/UiPath/Diamond/Project1/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9243" documentId="11_F9B9EC266AEF9A6C55FAC822FA75B080F77F927C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D808B5D7-F96B-4000-AF29-6FDC8BD4BEE6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Awarded" sheetId="3" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OpenBids!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Top5'!$A$1:$P$49</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -127,148 +128,145 @@
     <t>UOM</t>
   </si>
   <si>
+    <t>Download Link</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001816</t>
+  </si>
+  <si>
     <t>Quotation</t>
   </si>
   <si>
+    <t>Instructors for Digital Literacy Programme in Queenstown Secondary School</t>
+  </si>
+  <si>
     <t>Ministry of Education - Schools</t>
   </si>
   <si>
+    <t>14 Apr 2022 05:50PM</t>
+  </si>
+  <si>
+    <t>25 Apr 2022 01:00PM</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
+    <t>MR JOSEPH TEO</t>
+  </si>
+  <si>
+    <t>teo_chai_hong_joseph@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>1 Strathmore Road Singapore 148800</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001816</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001800</t>
+  </si>
+  <si>
+    <t>2022 English Bridging Support</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 05:05PM</t>
+  </si>
+  <si>
+    <t>GOH PAI SHEN</t>
+  </si>
+  <si>
+    <t>goh_pai_shen@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>Catholic High School (Secondary), 9 Bishan Street 22 Singapore 579767</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001800</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001802</t>
+  </si>
+  <si>
+    <t>ITQ for Supply of Instructor for Mother Tongue Fortnight activities for Students in Beacon Primary School for our P1-P6 students</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 04:05PM</t>
+  </si>
+  <si>
+    <t>MS LEE PEI PEI</t>
+  </si>
+  <si>
+    <t>lee_pei_pei@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>Ministry of Education,1, North Buona Vista Drive</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001802</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001811</t>
+  </si>
+  <si>
+    <t>Supply of Pianist for Choir CCA Programme in Clementi Primary School</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 03:35PM</t>
+  </si>
+  <si>
+    <t>FIONA KWAN</t>
+  </si>
+  <si>
+    <t>fiona_kwan_lok_mun@moe.edu.sg</t>
+  </si>
+  <si>
+    <t>8 Clementi Avenue 3 Singapore 129903</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001811</t>
+  </si>
+  <si>
+    <t>NYP000ETQ22000081</t>
+  </si>
+  <si>
+    <t>To appoint training service providers for the provision of services to develop and deliver Masterclass Programmes for a period of 2 years</t>
+  </si>
+  <si>
     <t>Nanyang Polytechnic</t>
   </si>
   <si>
-    <t>25 Apr 2022 01:00PM</t>
+    <t>14 Apr 2022 02:19PM</t>
+  </si>
+  <si>
+    <t>05 May 2022 01:00PM</t>
+  </si>
+  <si>
+    <t>JENNY LING / PATRICK PNG</t>
+  </si>
+  <si>
+    <t>jenny_ling@sirs.edu.sg</t>
+  </si>
+  <si>
+    <t>64173650 / 65500717</t>
+  </si>
+  <si>
+    <t>Singapore Institute of Retail Studies, 11 Eunos Road 8, Lifelong Learning Institute, #08-02/03/04, Singapore 408601</t>
+  </si>
+  <si>
+    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\NYP000ETQ22000081</t>
+  </si>
+  <si>
+    <t>MOESCHETQ22001805</t>
+  </si>
+  <si>
+    <t>Manpower service for Science Lab 1+1 year</t>
+  </si>
+  <si>
+    <t>14 Apr 2022 02:05PM</t>
   </si>
   <si>
     <t>04 May 2022 01:00PM</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Download Link</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001816</t>
-  </si>
-  <si>
-    <t>Instructors for Digital Literacy Programme in Queenstown Secondary School</t>
-  </si>
-  <si>
-    <t>14 Apr 2022 05:50PM</t>
-  </si>
-  <si>
-    <t>MR JOSEPH TEO</t>
-  </si>
-  <si>
-    <t>teo_chai_hong_joseph@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>1 Strathmore Road Singapore 148800</t>
-  </si>
-  <si>
-    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001816</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001800</t>
-  </si>
-  <si>
-    <t>2022 English Bridging Support</t>
-  </si>
-  <si>
-    <t>14 Apr 2022 05:05PM</t>
-  </si>
-  <si>
-    <t>GOH PAI SHEN</t>
-  </si>
-  <si>
-    <t>goh_pai_shen@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>Catholic High School (Secondary), 9 Bishan Street 22 Singapore 579767</t>
-  </si>
-  <si>
-    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001800</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001802</t>
-  </si>
-  <si>
-    <t>ITQ for Supply of Instructor for Mother Tongue Fortnight activities for Students in Beacon Primary School for our P1-P6 students</t>
-  </si>
-  <si>
-    <t>14 Apr 2022 04:05PM</t>
-  </si>
-  <si>
-    <t>MS LEE PEI PEI</t>
-  </si>
-  <si>
-    <t>lee_pei_pei@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>Ministry of Education,1, North Buona Vista Drive</t>
-  </si>
-  <si>
-    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001802</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001811</t>
-  </si>
-  <si>
-    <t>Supply of Pianist for Choir CCA Programme in Clementi Primary School</t>
-  </si>
-  <si>
-    <t>14 Apr 2022 03:35PM</t>
-  </si>
-  <si>
-    <t>FIONA KWAN</t>
-  </si>
-  <si>
-    <t>fiona_kwan_lok_mun@moe.edu.sg</t>
-  </si>
-  <si>
-    <t>8 Clementi Avenue 3 Singapore 129903</t>
-  </si>
-  <si>
-    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001811</t>
-  </si>
-  <si>
-    <t>NYP000ETQ22000081</t>
-  </si>
-  <si>
-    <t>To appoint training service providers for the provision of services to develop and deliver Masterclass Programmes for a period of 2 years</t>
-  </si>
-  <si>
-    <t>14 Apr 2022 02:19PM</t>
-  </si>
-  <si>
-    <t>05 May 2022 01:00PM</t>
-  </si>
-  <si>
-    <t>JENNY LING / PATRICK PNG</t>
-  </si>
-  <si>
-    <t>jenny_ling@sirs.edu.sg</t>
-  </si>
-  <si>
-    <t>64173650 / 65500717</t>
-  </si>
-  <si>
-    <t>Singapore Institute of Retail Studies, 11 Eunos Road 8, Lifelong Learning Institute, #08-02/03/04, Singapore 408601</t>
-  </si>
-  <si>
-    <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\NYP000ETQ22000081</t>
-  </si>
-  <si>
-    <t>MOESCHETQ22001805</t>
-  </si>
-  <si>
-    <t>Manpower service for Science Lab 1+1 year</t>
-  </si>
-  <si>
-    <t>14 Apr 2022 02:05PM</t>
   </si>
   <si>
     <t>MRS EMILY WONG</t>
@@ -382,6 +380,9 @@
   </si>
   <si>
     <t>C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001730</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
   <si>
     <t>MOESCHETQ22001462</t>
@@ -507,7 +508,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -967,7 +968,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -993,34 +993,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="131"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1032,34 +1032,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="131"/>
                 <c:pt idx="0">
-                  <c:v>398</c:v>
+                  <c:v>376</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>323</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>305</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>275</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>267</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>194</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>88</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,7 +1639,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1647,6 +1646,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill>
@@ -2587,21 +2587,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.77734375" style="1"/>
-    <col min="5" max="5" width="35.77734375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="4" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="35.81640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>109</v>
@@ -2641,7 +2641,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>113</v>
@@ -2661,7 +2661,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>117</v>
@@ -2681,7 +2681,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>121</v>
@@ -2701,7 +2701,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>125</v>
@@ -2721,7 +2721,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>129</v>
@@ -2741,7 +2741,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>132</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>133</v>
@@ -2761,7 +2761,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>136</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>137</v>
@@ -2781,7 +2781,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>140</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>141</v>
@@ -2801,7 +2801,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>144</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>145</v>
@@ -2827,26 +2827,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="1"/>
-    <col min="3" max="3" width="8.88671875" style="1" customWidth="1"/>
-    <col min="4" max="8" width="8.77734375" style="1"/>
-    <col min="9" max="9" width="6.109375" style="1" customWidth="1"/>
-    <col min="10" max="13" width="8.77734375" style="1"/>
-    <col min="14" max="16" width="14.77734375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="8.90625" style="1" customWidth="1"/>
+    <col min="4" max="8" width="8.81640625" style="1"/>
+    <col min="9" max="9" width="6.08984375" style="1" customWidth="1"/>
+    <col min="10" max="13" width="8.81640625" style="1"/>
+    <col min="14" max="16" width="14.81640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2896,42 +2896,42 @@
         <v>23</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="L2" s="1">
         <v>64741055</v>
@@ -2940,51 +2940,51 @@
         <v>64741295</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O2" s="1">
-        <v>267</v>
+        <v>341</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="L3" s="1">
         <v>64582177</v>
@@ -2993,51 +2993,51 @@
         <v>64561322</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1">
-        <v>398</v>
+        <v>114</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="L4" s="1">
         <v>67697255</v>
@@ -3046,151 +3046,151 @@
         <v>67697244</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O4" s="1">
-        <v>275</v>
+        <v>110</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="L5" s="1">
         <v>67797449</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O5" s="1">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="O6" s="1">
+        <v>112</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="1">
-        <v>323</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="L7" s="1">
         <v>68962054</v>
@@ -3199,51 +3199,51 @@
         <v>65632356</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="1">
+        <v>244</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="1">
-        <v>75</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="L8" s="1">
         <v>62886516</v>
@@ -3252,51 +3252,51 @@
         <v>62876393</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="1">
+        <v>290</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="1">
-        <v>88</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="L9" s="1">
         <v>62886516</v>
@@ -3305,51 +3305,51 @@
         <v>62876393</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="1">
+        <v>104</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O9" s="1">
-        <v>82</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="L10" s="1">
         <v>63443072</v>
@@ -3358,101 +3358,101 @@
         <v>63459007</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O10" s="1">
+        <v>284</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O10" s="1">
-        <v>194</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="L11" s="1">
         <v>67932039</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O11" s="1">
+        <v>158</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O11" s="1">
-        <v>61</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="L12" s="1">
         <v>62575684</v>
@@ -3461,16 +3461,16 @@
         <v>67558802</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12" s="1">
+        <v>376</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="O12" s="1">
-        <v>305</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3479,21 +3479,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="13" width="8.77734375" style="1"/>
-    <col min="14" max="14" width="14.77734375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="13" width="8.81640625" style="1"/>
+    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3543,536 +3543,534 @@
         <v>23</v>
       </c>
       <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2">
+        <v>62575684</v>
+      </c>
+      <c r="M2">
+        <v>67558802</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2">
+        <v>376</v>
+      </c>
+      <c r="P2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3">
+        <v>64741055</v>
+      </c>
+      <c r="M3">
+        <v>64741295</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3">
+        <v>341</v>
+      </c>
+      <c r="P3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2">
-        <v>64582177</v>
-      </c>
-      <c r="M2">
-        <v>64561322</v>
-      </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2">
-        <v>398</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4">
+        <v>62886516</v>
+      </c>
+      <c r="M4">
+        <v>62876393</v>
+      </c>
+      <c r="N4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4">
+        <v>290</v>
+      </c>
+      <c r="P4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3"/>
-      <c r="N3" t="s">
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5">
+        <v>63443072</v>
+      </c>
+      <c r="M5">
+        <v>63459007</v>
+      </c>
+      <c r="N5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5">
+        <v>284</v>
+      </c>
+      <c r="P5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="O3">
-        <v>323</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6">
+        <v>68962054</v>
+      </c>
+      <c r="M6">
+        <v>65632356</v>
+      </c>
+      <c r="N6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6">
+        <v>244</v>
+      </c>
+      <c r="P6" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7">
+        <v>67797449</v>
+      </c>
+      <c r="M7"/>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7">
+        <v>206</v>
+      </c>
+      <c r="P7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" t="s">
-        <v>105</v>
-      </c>
-      <c r="L4">
-        <v>62575684</v>
-      </c>
-      <c r="M4">
-        <v>67558802</v>
-      </c>
-      <c r="N4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O4">
-        <v>305</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="G8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5">
-        <v>67697255</v>
-      </c>
-      <c r="M5">
-        <v>67697244</v>
-      </c>
-      <c r="N5" t="s">
-        <v>51</v>
-      </c>
-      <c r="O5">
-        <v>275</v>
-      </c>
-      <c r="P5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6">
-        <v>64741055</v>
-      </c>
-      <c r="M6">
-        <v>64741295</v>
-      </c>
-      <c r="N6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O6">
-        <v>267</v>
-      </c>
-      <c r="P6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K7" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7">
-        <v>63443072</v>
-      </c>
-      <c r="M7">
-        <v>63459007</v>
-      </c>
-      <c r="N7" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7">
-        <v>194</v>
-      </c>
-      <c r="P7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="K8" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="L8">
-        <v>67797449</v>
+        <v>67932039</v>
       </c>
       <c r="M8"/>
       <c r="N8" t="s">
+        <v>99</v>
+      </c>
+      <c r="O8">
+        <v>158</v>
+      </c>
+      <c r="P8" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <v>64582177</v>
+      </c>
+      <c r="M9">
+        <v>64561322</v>
+      </c>
+      <c r="N9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9">
+        <v>114</v>
+      </c>
+      <c r="P9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="O8">
-        <v>94</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10">
+        <v>112</v>
+      </c>
+      <c r="P10" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" t="s">
-        <v>80</v>
-      </c>
-      <c r="L9">
-        <v>62886516</v>
-      </c>
-      <c r="M9">
-        <v>62876393</v>
-      </c>
-      <c r="N9" t="s">
-        <v>81</v>
-      </c>
-      <c r="O9">
-        <v>88</v>
-      </c>
-      <c r="P9" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" t="s">
-        <v>87</v>
-      </c>
-      <c r="L10">
-        <v>62886516</v>
-      </c>
-      <c r="M10">
-        <v>62876393</v>
-      </c>
-      <c r="N10" t="s">
-        <v>88</v>
-      </c>
-      <c r="O10">
-        <v>82</v>
-      </c>
-      <c r="P10" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J11" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="L11">
-        <v>68962054</v>
+        <v>67697255</v>
       </c>
       <c r="M11">
-        <v>65632356</v>
+        <v>67697244</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="O11">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="P11" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="Q11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -4091,7 +4089,7 @@
       <c r="P12"/>
       <c r="Q12"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -4108,8 +4106,9 @@
       <c r="N13"/>
       <c r="O13"/>
       <c r="P13"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -4126,8 +4125,9 @@
       <c r="N14"/>
       <c r="O14"/>
       <c r="P14"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -4144,8 +4144,9 @@
       <c r="N15"/>
       <c r="O15"/>
       <c r="P15"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -4162,8 +4163,9 @@
       <c r="N16"/>
       <c r="O16"/>
       <c r="P16"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -4180,8 +4182,9 @@
       <c r="N17"/>
       <c r="O17"/>
       <c r="P17"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -4198,8 +4201,9 @@
       <c r="N18"/>
       <c r="O18"/>
       <c r="P18"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -4216,8 +4220,9 @@
       <c r="N19"/>
       <c r="O19"/>
       <c r="P19"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -4234,8 +4239,9 @@
       <c r="N20"/>
       <c r="O20"/>
       <c r="P20"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -4252,8 +4258,9 @@
       <c r="N21"/>
       <c r="O21"/>
       <c r="P21"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -4270,8 +4277,9 @@
       <c r="N22"/>
       <c r="O22"/>
       <c r="P22"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -4288,8 +4296,9 @@
       <c r="N23"/>
       <c r="O23"/>
       <c r="P23"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -4306,8 +4315,9 @@
       <c r="N24"/>
       <c r="O24"/>
       <c r="P24"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -4324,8 +4334,9 @@
       <c r="N25"/>
       <c r="O25"/>
       <c r="P25"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -4342,8 +4353,9 @@
       <c r="N26"/>
       <c r="O26"/>
       <c r="P26"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -4360,8 +4372,9 @@
       <c r="N27"/>
       <c r="O27"/>
       <c r="P27"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -4378,8 +4391,9 @@
       <c r="N28"/>
       <c r="O28"/>
       <c r="P28"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -4396,8 +4410,9 @@
       <c r="N29"/>
       <c r="O29"/>
       <c r="P29"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -4414,8 +4429,9 @@
       <c r="N30"/>
       <c r="O30"/>
       <c r="P30"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -4433,7 +4449,7 @@
       <c r="O31"/>
       <c r="P31"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -4451,7 +4467,7 @@
       <c r="O32"/>
       <c r="P32"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -4469,7 +4485,7 @@
       <c r="O33"/>
       <c r="P33"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -4487,7 +4503,7 @@
       <c r="O34"/>
       <c r="P34"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -4505,7 +4521,7 @@
       <c r="O35"/>
       <c r="P35"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -4523,7 +4539,7 @@
       <c r="O36"/>
       <c r="P36"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -4541,7 +4557,7 @@
       <c r="O37"/>
       <c r="P37"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -4559,7 +4575,7 @@
       <c r="O38"/>
       <c r="P38"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -4577,7 +4593,7 @@
       <c r="O39"/>
       <c r="P39"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -4595,7 +4611,7 @@
       <c r="O40"/>
       <c r="P40"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -4613,7 +4629,7 @@
       <c r="O41"/>
       <c r="P41"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -4631,7 +4647,7 @@
       <c r="O42"/>
       <c r="P42"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -4649,7 +4665,7 @@
       <c r="O43"/>
       <c r="P43"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -4667,7 +4683,7 @@
       <c r="O44"/>
       <c r="P44"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -4685,7 +4701,7 @@
       <c r="O45"/>
       <c r="P45"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -4703,7 +4719,7 @@
       <c r="O46"/>
       <c r="P46"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -4721,7 +4737,7 @@
       <c r="O47"/>
       <c r="P47"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -4739,7 +4755,7 @@
       <c r="O48"/>
       <c r="P48"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -4757,7 +4773,7 @@
       <c r="O49"/>
       <c r="P49"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -4775,7 +4791,7 @@
       <c r="O50"/>
       <c r="P50"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -4793,7 +4809,7 @@
       <c r="O51"/>
       <c r="P51"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -4811,7 +4827,7 @@
       <c r="O52"/>
       <c r="P52"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -4829,7 +4845,7 @@
       <c r="O53"/>
       <c r="P53"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -4847,7 +4863,7 @@
       <c r="O54"/>
       <c r="P54"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -4865,7 +4881,7 @@
       <c r="O55"/>
       <c r="P55"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -4883,7 +4899,7 @@
       <c r="O56"/>
       <c r="P56"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -4901,7 +4917,7 @@
       <c r="O57"/>
       <c r="P57"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -4919,7 +4935,7 @@
       <c r="O58"/>
       <c r="P58"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -4937,7 +4953,7 @@
       <c r="O59"/>
       <c r="P59"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -4955,7 +4971,7 @@
       <c r="O60"/>
       <c r="P60"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -4973,7 +4989,7 @@
       <c r="O61"/>
       <c r="P61"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -4991,7 +5007,7 @@
       <c r="O62"/>
       <c r="P62"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -5009,7 +5025,7 @@
       <c r="O63"/>
       <c r="P63"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -5027,7 +5043,7 @@
       <c r="O64"/>
       <c r="P64"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -5045,7 +5061,7 @@
       <c r="O65"/>
       <c r="P65"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -5063,7 +5079,7 @@
       <c r="O66"/>
       <c r="P66"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -5081,7 +5097,7 @@
       <c r="O67"/>
       <c r="P67"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -5099,7 +5115,7 @@
       <c r="O68"/>
       <c r="P68"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -5117,7 +5133,7 @@
       <c r="O69"/>
       <c r="P69"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -5135,7 +5151,7 @@
       <c r="O70"/>
       <c r="P70"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -5153,7 +5169,7 @@
       <c r="O71"/>
       <c r="P71"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -5171,7 +5187,7 @@
       <c r="O72"/>
       <c r="P72"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -5189,7 +5205,7 @@
       <c r="O73"/>
       <c r="P73"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -5207,7 +5223,7 @@
       <c r="O74"/>
       <c r="P74"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -5225,7 +5241,7 @@
       <c r="O75"/>
       <c r="P75"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -5243,7 +5259,7 @@
       <c r="O76"/>
       <c r="P76"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -5261,7 +5277,7 @@
       <c r="O77"/>
       <c r="P77"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -5279,7 +5295,7 @@
       <c r="O78"/>
       <c r="P78"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -5297,7 +5313,7 @@
       <c r="O79"/>
       <c r="P79"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -5315,7 +5331,7 @@
       <c r="O80"/>
       <c r="P80"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -5333,7 +5349,7 @@
       <c r="O81"/>
       <c r="P81"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -5351,7 +5367,7 @@
       <c r="O82"/>
       <c r="P82"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -5369,7 +5385,7 @@
       <c r="O83"/>
       <c r="P83"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -5387,7 +5403,7 @@
       <c r="O84"/>
       <c r="P84"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -5405,7 +5421,7 @@
       <c r="O85"/>
       <c r="P85"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -5423,7 +5439,7 @@
       <c r="O86"/>
       <c r="P86"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -5441,7 +5457,7 @@
       <c r="O87"/>
       <c r="P87"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -5459,7 +5475,7 @@
       <c r="O88"/>
       <c r="P88"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -5477,7 +5493,7 @@
       <c r="O89"/>
       <c r="P89"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -5495,7 +5511,7 @@
       <c r="O90"/>
       <c r="P90"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -5513,7 +5529,7 @@
       <c r="O91"/>
       <c r="P91"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -5531,7 +5547,7 @@
       <c r="O92"/>
       <c r="P92"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -5549,7 +5565,7 @@
       <c r="O93"/>
       <c r="P93"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -5567,7 +5583,7 @@
       <c r="O94"/>
       <c r="P94"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -5585,7 +5601,7 @@
       <c r="O95"/>
       <c r="P95"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -5603,7 +5619,7 @@
       <c r="O96"/>
       <c r="P96"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -5621,7 +5637,7 @@
       <c r="O97"/>
       <c r="P97"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -5639,7 +5655,7 @@
       <c r="O98"/>
       <c r="P98"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -5657,7 +5673,7 @@
       <c r="O99"/>
       <c r="P99"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -5675,7 +5691,7 @@
       <c r="O100"/>
       <c r="P100"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -5693,7 +5709,7 @@
       <c r="O101"/>
       <c r="P101"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -5711,7 +5727,7 @@
       <c r="O102"/>
       <c r="P102"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -5729,7 +5745,7 @@
       <c r="O103"/>
       <c r="P103"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -5747,7 +5763,7 @@
       <c r="O104"/>
       <c r="P104"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -5765,7 +5781,7 @@
       <c r="O105"/>
       <c r="P105"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -5783,7 +5799,7 @@
       <c r="O106"/>
       <c r="P106"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -5801,7 +5817,7 @@
       <c r="O107"/>
       <c r="P107"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -5819,7 +5835,7 @@
       <c r="O108"/>
       <c r="P108"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -5837,7 +5853,7 @@
       <c r="O109"/>
       <c r="P109"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -5855,7 +5871,7 @@
       <c r="O110"/>
       <c r="P110"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -5873,7 +5889,7 @@
       <c r="O111"/>
       <c r="P111"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -5891,7 +5907,7 @@
       <c r="O112"/>
       <c r="P112"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
@@ -5909,7 +5925,7 @@
       <c r="O113"/>
       <c r="P113"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -5927,7 +5943,7 @@
       <c r="O114"/>
       <c r="P114"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
@@ -5945,7 +5961,7 @@
       <c r="O115"/>
       <c r="P115"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -5963,7 +5979,7 @@
       <c r="O116"/>
       <c r="P116"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -5981,7 +5997,7 @@
       <c r="O117"/>
       <c r="P117"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -5999,7 +6015,7 @@
       <c r="O118"/>
       <c r="P118"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -6017,7 +6033,7 @@
       <c r="O119"/>
       <c r="P119"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -6035,7 +6051,7 @@
       <c r="O120"/>
       <c r="P120"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
@@ -6053,7 +6069,7 @@
       <c r="O121"/>
       <c r="P121"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
@@ -6071,7 +6087,7 @@
       <c r="O122"/>
       <c r="P122"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -6089,7 +6105,7 @@
       <c r="O123"/>
       <c r="P123"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
@@ -6107,7 +6123,7 @@
       <c r="O124"/>
       <c r="P124"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
@@ -6125,7 +6141,7 @@
       <c r="O125"/>
       <c r="P125"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
@@ -6143,7 +6159,7 @@
       <c r="O126"/>
       <c r="P126"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -6161,7 +6177,7 @@
       <c r="O127"/>
       <c r="P127"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
@@ -6179,7 +6195,7 @@
       <c r="O128"/>
       <c r="P128"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
@@ -6197,7 +6213,7 @@
       <c r="O129"/>
       <c r="P129"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -6215,7 +6231,7 @@
       <c r="O130"/>
       <c r="P130"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -6233,7 +6249,7 @@
       <c r="O131"/>
       <c r="P131"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -6241,27 +6257,27 @@
       <c r="E132"/>
     </row>
   </sheetData>
-  <sortState ref="A2:Q132">
-    <sortCondition descending="1" ref="O1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q132">
+    <sortCondition descending="1" ref="O1:O132"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="2" spans="2:15" ht="46" x14ac:dyDescent="1">
       <c r="B2" s="38" t="s">
         <v>20</v>
       </c>
@@ -6279,7 +6295,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B4" s="43" t="s">
         <v>2</v>
       </c>
@@ -6296,7 +6312,7 @@
       <c r="K4" s="50"/>
       <c r="L4" s="51"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -6307,7 +6323,7 @@
       <c r="K6" s="17"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
@@ -6318,7 +6334,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="2:15" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="8" spans="2:15" ht="46" x14ac:dyDescent="1">
       <c r="B8" s="6"/>
       <c r="C8" s="9">
         <f>COUNT(OpenBids!A:A)</f>
@@ -6338,7 +6354,7 @@
       </c>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
@@ -6349,7 +6365,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
@@ -6360,14 +6376,14 @@
       <c r="K10" s="24"/>
       <c r="L10" s="25"/>
     </row>
-    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="46" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="48"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="26" t="s">
         <v>5</v>
       </c>
@@ -6388,19 +6404,19 @@
       </c>
       <c r="L13" s="41"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="27">
         <f>'Top5'!A2</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C14" s="28" t="str">
         <f>'Top5'!B2</f>
-        <v>MOESCHETQ22001800</v>
+        <v>MOESCHETQ22001730</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="35" t="str">
         <f>'Top5'!E2</f>
-        <v>2022 English Bridging Support</v>
+        <v>Supply of Instructors for Primary 1 Programme for Active Learning (PAL) - Dance Module in Peiying Primary School</v>
       </c>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
@@ -6413,19 +6429,19 @@
       </c>
       <c r="L14" s="29"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" s="27">
         <f>'Top5'!A3</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15" s="28" t="str">
         <f>'Top5'!B3</f>
-        <v>NYP000ETQ22000081</v>
+        <v>MOESCHETQ22001816</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="35" t="str">
         <f>'Top5'!E3</f>
-        <v>To appoint training service providers for the provision of services to develop and deliver Masterclass Programmes for a period of 2 years</v>
+        <v>Instructors for Digital Literacy Programme in Queenstown Secondary School</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
@@ -6434,23 +6450,23 @@
       <c r="J15" s="37"/>
       <c r="K15" s="31" t="str">
         <f>'Top5'!H3</f>
-        <v>05 May 2022 01:00PM</v>
+        <v>25 Apr 2022 01:00PM</v>
       </c>
       <c r="L15" s="29"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="27">
         <f>'Top5'!A4</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C16" s="28" t="str">
         <f>'Top5'!B4</f>
-        <v>MOESCHETQ22001730</v>
+        <v>MOESCHETQ22001795</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="35" t="str">
         <f>'Top5'!E4</f>
-        <v>Supply of Instructors for Primary 1 Programme for Active Learning (PAL) - Dance Module in Peiying Primary School</v>
+        <v>Provision of 3 Days Non-Residential Primary 5 Cohort Outdoor Learning Camp 2022</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -6463,19 +6479,19 @@
       </c>
       <c r="L16" s="29"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="27">
         <f>'Top5'!A5</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C17" s="28" t="str">
         <f>'Top5'!B5</f>
-        <v>MOESCHETQ22001802</v>
+        <v>MOESCHETQ22001791</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="35" t="str">
         <f>'Top5'!E5</f>
-        <v>ITQ for Supply of Instructor for Mother Tongue Fortnight activities for Students in Beacon Primary School for our P1-P6 students</v>
+        <v>Supply of Instructor for Student Leadership Programme for CHIJ (Katong) Primary: - P4 to P6 Prefects (Trainee &amp; Senior) and P3 to P6 Class Monitors</v>
       </c>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
@@ -6488,19 +6504,19 @@
       </c>
       <c r="L17" s="29"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="27">
         <f>'Top5'!A6</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C18" s="28" t="str">
         <f>'Top5'!B6</f>
-        <v>MOESCHETQ22001816</v>
+        <v>MOESCHETQ22001805</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="32" t="str">
         <f>'Top5'!E6</f>
-        <v>Instructors for Digital Literacy Programme in Queenstown Secondary School</v>
+        <v>Manpower service for Science Lab 1+1 year</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
@@ -6509,11 +6525,11 @@
       <c r="J18" s="34"/>
       <c r="K18" s="31" t="str">
         <f>'Top5'!H6</f>
-        <v>25 Apr 2022 01:00PM</v>
+        <v>04 May 2022 01:00PM</v>
       </c>
       <c r="L18" s="29"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>

</xml_diff>